<commit_message>
Finish ortholog prediction and the plotting codes for each group.
Finish ortholog prediction and fill all the excel table. Add the rest of
groups (eg. Clock4) in my R script.
</commit_message>
<xml_diff>
--- a/circadian_gene_orthologs_v2.xlsx
+++ b/circadian_gene_orthologs_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Po-Kai\Box Sync\Mimulus_swc_timecourse_2018\RNAseq\limma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06374E9A-2368-470B-B863-A7BAC4E2E6E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BFC54F-ADE5-4E12-BA81-DAF913C2C6A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{93B91BF5-8888-4255-9D7D-6B7A94E49BDB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="86">
   <si>
     <t>Arabidopsis_genes</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,177 @@
   </si>
   <si>
     <t>Q8L500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIF5</t>
+  </si>
+  <si>
+    <t>Q84LH8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT3G59060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ELF3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT2G25930</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O82804</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clock4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ELF4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT2G40080</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O04211</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.F01385</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.N00783</t>
+  </si>
+  <si>
+    <t>LUX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT3G46640</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q9SNB4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.D00884</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.E01551</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT5G15840</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q39057</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.H00566</t>
+  </si>
+  <si>
+    <t>F_photoperiod</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.A00403</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.E01434</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT1G22770</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q9SQI2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.N02951</t>
+  </si>
+  <si>
+    <t>Migut.C00380</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FKF1</t>
+  </si>
+  <si>
+    <t>AT1G68050</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q9C9W9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.E00487</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT1G65480</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q9SXZ2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.F01843</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.F02091</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.F02093</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.G00570</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HEMERA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT2G34640</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F4IHY7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Migut.M01863</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -197,7 +368,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,6 +381,14 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -236,12 +415,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DC3834-7083-4E97-9028-BD929471FD15}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -792,6 +974,278 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>